<commit_message>
catalogos completos y pocas validaciones
</commit_message>
<xml_diff>
--- a/PENDIENTES 2025-04-10.xlsx
+++ b/PENDIENTES 2025-04-10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plastictrendsmx-my.sharepoint.com/personal/juan_garcia_plastictrends_com_mx/Documents/Personal/PROYECTOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MYCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{755020C2-A22D-458F-AE31-2D753EBC3DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1532FA80-57DB-440D-B531-9AC6D4ABA295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBC73E7B-1B67-4EE4-BD47-9A1CA65E3A83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBC73E7B-1B67-4EE4-BD47-9A1CA65E3A83}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>INICIO</t>
   </si>
@@ -201,13 +201,16 @@
   </si>
   <si>
     <t>cierre de soporte con firma del cliente en tablet</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,13 +234,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,13 +268,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,25 +610,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E258A968-40E9-4235-8250-A55D416219E6}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B65"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="90.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="2" width="90.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="20.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -619,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -627,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -635,12 +652,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="20.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -648,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -656,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -664,7 +681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -672,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -680,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -688,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -696,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -704,28 +721,34 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="20.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="18.75">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.75">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -733,7 +756,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -741,7 +764,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -749,7 +772,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -757,7 +780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -765,7 +788,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -773,12 +796,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -786,7 +809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -794,12 +817,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -807,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -815,7 +838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -823,12 +846,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -836,7 +859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -844,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -852,7 +875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -860,7 +883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -868,12 +891,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -881,7 +904,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -889,7 +912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -897,12 +920,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15">
       <c r="A47" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -910,7 +933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -918,12 +941,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15">
       <c r="A51" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -931,12 +954,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15">
       <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -944,27 +967,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="20.25">
       <c r="A58" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="B59" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="B60" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="B61" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -972,7 +995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -980,17 +1003,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="B64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nuevos OK resueltos en excel
</commit_message>
<xml_diff>
--- a/PENDIENTES 2025-04-10.xlsx
+++ b/PENDIENTES 2025-04-10.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MYCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1532FA80-57DB-440D-B531-9AC6D4ABA295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30167B9B-6B1B-4E58-96BD-22BFF380E8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBC73E7B-1B67-4EE4-BD47-9A1CA65E3A83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBC73E7B-1B67-4EE4-BD47-9A1CA65E3A83}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>INICIO</t>
   </si>
@@ -210,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,23 +612,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E258A968-40E9-4235-8250-A55D416219E6}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="2" width="90.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="4.125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -644,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -652,12 +652,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.25">
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -673,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -681,7 +681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -689,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -697,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -705,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -713,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -721,12 +721,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="20.25">
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18.75">
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -737,7 +737,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75">
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -748,7 +748,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -756,23 +756,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -780,15 +786,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -796,12 +805,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -809,7 +818,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -817,12 +826,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -830,7 +839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -838,7 +847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -846,20 +855,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>15</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -867,7 +879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -875,7 +887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -883,7 +895,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -891,28 +903,34 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>15</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -920,12 +938,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -933,20 +951,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15">
+      <c r="C49" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -954,40 +975,43 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="20.25">
+      <c r="C55" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -995,7 +1019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -1003,12 +1027,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>54</v>
       </c>

</xml_diff>